<commit_message>
Update Deposit and Withdrawl Method Implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="930" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="930" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="6" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="openAccountTest" sheetId="4" r:id="rId4"/>
     <sheet name="Validatecustomers" sheetId="5" r:id="rId5"/>
     <sheet name="customerloginTest" sheetId="7" r:id="rId6"/>
-    <sheet name="amountwithdrawlTest" sheetId="8" r:id="rId7"/>
-    <sheet name="amountDepositTest" sheetId="9" r:id="rId8"/>
+    <sheet name="amountDepositTest" sheetId="9" r:id="rId7"/>
+    <sheet name="amountwithdrawlTest" sheetId="8" r:id="rId8"/>
     <sheet name="amountTransactionDetailsTest" sheetId="12" r:id="rId9"/>
     <sheet name="customerLogoutTest" sheetId="10" r:id="rId10"/>
   </sheets>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="34">
   <si>
     <t>username</t>
   </si>
@@ -87,12 +87,6 @@
   </si>
   <si>
     <t>customerloginTest</t>
-  </si>
-  <si>
-    <t>DepositAmount</t>
-  </si>
-  <si>
-    <t>WithDrawlAmount</t>
   </si>
   <si>
     <t>Dharmendra</t>
@@ -514,7 +508,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +527,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -573,7 +567,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -581,7 +575,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -589,15 +583,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -631,7 +625,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -669,7 +663,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -692,7 +686,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,10 +711,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1234</v>
@@ -731,10 +725,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>4212</v>
@@ -774,7 +768,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -817,10 +811,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>4212</v>
@@ -857,7 +851,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -871,10 +865,74 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>700</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +946,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -896,12 +954,34 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>400</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -911,53 +991,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2">
-        <v>300</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -973,13 +1011,13 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
         <v>9</v>
@@ -987,36 +1025,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3">
         <v>300</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>